<commit_message>
Archivo con nuestras estaciones.
</commit_message>
<xml_diff>
--- a/Matchups/matchupsdeturbidez/L7.xlsx
+++ b/Matchups/matchupsdeturbidez/L7.xlsx
@@ -46,6 +46,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -148,12 +149,12 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>